<commit_message>
Atualizando página about me
</commit_message>
<xml_diff>
--- a/documentacao/requisitos-blank-paper.xlsx
+++ b/documentacao/requisitos-blank-paper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberta\Desktop\projeto-individual-site\blank-paper\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1C055C-28FA-48DF-8D24-986A8BCC1EE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF68054-94C8-4C55-8549-01B0938392D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FC8E7A36-AF2F-4BA9-B3C7-600CAFE632A5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID </t>
   </si>
@@ -94,9 +94,6 @@
     <t>Criar páginas de Login e Cadastro para o site (Front-End).</t>
   </si>
   <si>
-    <t>Criar e manipular o sensor para os propósitos do projeto.</t>
-  </si>
-  <si>
     <t>Apresentar o projeto para a banca.</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
  "index.html", "about-me.html", "my-works.html", "contact.html" e "login.html".</t>
   </si>
   <si>
-    <t xml:space="preserve">Desenvolver o Banco de Dados que contém as tabelas: "usuario" e "contatos". </t>
-  </si>
-  <si>
     <t>Desenvolver o metódo onde a venda de comissões de desenhos será feita.</t>
   </si>
   <si>
@@ -137,14 +131,29 @@
     <t>Apresentar esses dados coletados no banco de dados.</t>
   </si>
   <si>
-    <t>Criar lógica para verificar Cadastros e Logins e validação da textarea. (Back-End).</t>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolver o Banco de Dados que contém as tabelas: "usuario" e "comissoes". </t>
+  </si>
+  <si>
+    <t>Criar lógica para verificar Cadastros e Logins e validação da página de contact. (Back-End).</t>
+  </si>
+  <si>
+    <t>Manipular o a inserção das comissões no site para os propósitos do projeto.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,31 +162,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Biome"/>
+      <name val="Daytona"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Daytona"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Biome"/>
+      <name val="Daytona"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFAFAFA"/>
-      <name val="Biome"/>
+      <name val="Daytona"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,13 +200,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3D5D17"/>
+        <fgColor rgb="FF293D0F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF293D0F"/>
+        <fgColor rgb="FFA1D75F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2B4010"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -229,19 +249,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -253,6 +273,7 @@
   <colors>
     <mruColors>
       <color rgb="FF2B4010"/>
+      <color rgb="FFA1D75F"/>
       <color rgb="FF365014"/>
       <color rgb="FF293D0F"/>
       <color rgb="FF1D2B0B"/>
@@ -567,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD617AA-C211-40D1-95CB-C51ABBB11CB1}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,286 +606,354 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5">
+        <f>SUM(D4:D6)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5">
+        <f>SUM(D9:D12)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5">
+        <v>21</v>
+      </c>
+      <c r="E17" s="5">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5">
+        <f>SUM(D15:D19)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5">
+        <v>8</v>
+      </c>
+      <c r="E19" s="5">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="3">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="3">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1">
-        <v>13</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1">
-        <v>15</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="3">
-        <f>SUM(D2:D13)</f>
+      <c r="F19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="6">
+        <f>SUM(D4:D19)</f>
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>